<commit_message>
Bot5 GUI no aparece el error en Cris PC
</commit_message>
<xml_diff>
--- a/Migraciones/ASIG-NDOC.xlsx
+++ b/Migraciones/ASIG-NDOC.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="851" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="DISPAZ" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="AG. ACHUMANI" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="AG. MURILLO" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="AG. MAX PAREDES" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="DISALTO" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="AG. SATELITE" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="DISCRUZ" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="AG. MUTUALISTA" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="AG. MONTERO" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="AG. WARNES" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="DISTAR" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="AG. TARIJEÑITA" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="COCHABAMBA" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="AG. HONDURAS" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="AG. CALAMA" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="SUCRE" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="AG. SUCRE 1" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="AG. SUCRE 2" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="POTOSI" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="AG. POTOSI 1" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="ORURO" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="AG. ORURO 1" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="TRINIDAD" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="AG. TRINIDAD 1" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="PANDO" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="RIBERALTA" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="IVSA" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="OPAL" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DISPAZ" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. ACHUMANI" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. MURILLO" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. MAX PAREDES" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DISALTO" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. SATELITE" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DISCRUZ" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. MUTUALISTA" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. MONTERO" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. WARNES" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DISTAR" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. TARIJEÑITA" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COCHABAMBA" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. HONDURAS" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. CALAMA" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SUCRE" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. SUCRE 1" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. SUCRE 2" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="POTOSI" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. POTOSI 1" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ORURO" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. ORURO 1" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRINIDAD" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AG. TRINIDAD 1" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PANDO" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RIBERALTA" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IVSA" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OPAL" sheetId="28" state="visible" r:id="rId28"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>0</col>
@@ -178,24 +178,24 @@
       <nvPicPr>
         <cNvPr id="32" name="Imagen 31"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="145075276"/>
           <a:ext cx="3724275" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -219,24 +219,24 @@
       <nvPicPr>
         <cNvPr id="33" name="Imagen 32"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="138598275"/>
           <a:ext cx="3724275" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -260,24 +260,24 @@
       <nvPicPr>
         <cNvPr id="34" name="Imagen 33"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="135150225"/>
           <a:ext cx="3695700" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -301,24 +301,24 @@
       <nvPicPr>
         <cNvPr id="36" name="Imagen 35"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId4"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="138979275"/>
           <a:ext cx="3695700" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -342,24 +342,24 @@
       <nvPicPr>
         <cNvPr id="35" name="Imagen 34"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId5"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="153142951"/>
           <a:ext cx="3733800" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -383,24 +383,24 @@
       <nvPicPr>
         <cNvPr id="37" name="Imagen 36"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId6"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="157333950"/>
           <a:ext cx="3714750" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -424,24 +424,24 @@
       <nvPicPr>
         <cNvPr id="38" name="Imagen 37"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId7"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="161143950"/>
           <a:ext cx="3714750" cy="152400"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -465,24 +465,24 @@
       <nvPicPr>
         <cNvPr id="39" name="Imagen 38"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId8"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="166477951"/>
           <a:ext cx="3705225" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -506,24 +506,24 @@
       <nvPicPr>
         <cNvPr id="40" name="Imagen 39"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId9"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="172031026"/>
           <a:ext cx="3714750" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -547,24 +547,24 @@
       <nvPicPr>
         <cNvPr id="41" name="Imagen 40"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId10"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="176222026"/>
           <a:ext cx="3724275" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -588,24 +588,24 @@
       <nvPicPr>
         <cNvPr id="42" name="Imagen 41"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId11"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="179670075"/>
           <a:ext cx="3724275" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -629,24 +629,24 @@
       <nvPicPr>
         <cNvPr id="43" name="Imagen 42"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId12"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="191109601"/>
           <a:ext cx="3724275" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -670,24 +670,24 @@
       <nvPicPr>
         <cNvPr id="44" name="Imagen 43"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId13"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="203501625"/>
           <a:ext cx="3705225" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -711,24 +711,24 @@
       <nvPicPr>
         <cNvPr id="46" name="Imagen 45"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId14"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="212836124"/>
           <a:ext cx="3714750" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -752,24 +752,24 @@
       <nvPicPr>
         <cNvPr id="45" name="Imagen 44"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId15"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="215903175"/>
           <a:ext cx="3714750" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -793,24 +793,24 @@
       <nvPicPr>
         <cNvPr id="47" name="Imagen 46"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId16"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="217808175"/>
           <a:ext cx="3705225" cy="152400"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -834,24 +834,24 @@
       <nvPicPr>
         <cNvPr id="48" name="Imagen 47"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId17"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="221427676"/>
           <a:ext cx="3724275" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -875,24 +875,24 @@
       <nvPicPr>
         <cNvPr id="49" name="Imagen 48"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId18"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="230190675"/>
           <a:ext cx="3705225" cy="152400"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -916,24 +916,24 @@
       <nvPicPr>
         <cNvPr id="50" name="Imagen 49"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId19"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="223170750"/>
           <a:ext cx="6210300" cy="514350"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -957,24 +957,24 @@
       <nvPicPr>
         <cNvPr id="52" name="Imagen 51"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId20"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="222418275"/>
           <a:ext cx="6219825" cy="504825"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -998,24 +998,24 @@
       <nvPicPr>
         <cNvPr id="53" name="Imagen 52"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId21"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="218217750"/>
           <a:ext cx="6219825" cy="352425"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1039,24 +1039,24 @@
       <nvPicPr>
         <cNvPr id="51" name="Imagen 50"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId22"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="236305725"/>
           <a:ext cx="3714750" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1080,24 +1080,24 @@
       <nvPicPr>
         <cNvPr id="54" name="Imagen 53"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId23"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="258403725"/>
           <a:ext cx="3724275" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1121,24 +1121,24 @@
       <nvPicPr>
         <cNvPr id="55" name="Imagen 54"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId24"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="254603250"/>
           <a:ext cx="3724275" cy="152400"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1162,24 +1162,24 @@
       <nvPicPr>
         <cNvPr id="56" name="Imagen 55"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId25"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="252498225"/>
           <a:ext cx="3705225" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1203,24 +1203,24 @@
       <nvPicPr>
         <cNvPr id="57" name="Imagen 56"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId26"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="248154825"/>
           <a:ext cx="3714750" cy="180975"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1244,24 +1244,24 @@
       <nvPicPr>
         <cNvPr id="58" name="Imagen 57"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId27"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="242839875"/>
           <a:ext cx="3714750" cy="152400"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1285,24 +1285,24 @@
       <nvPicPr>
         <cNvPr id="59" name="Imagen 58"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId28"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="263623425"/>
           <a:ext cx="3705225" cy="180975"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1326,24 +1326,24 @@
       <nvPicPr>
         <cNvPr id="60" name="Imagen 59"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId29"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="271052925"/>
           <a:ext cx="3714750" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1367,24 +1367,24 @@
       <nvPicPr>
         <cNvPr id="61" name="Imagen 60"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId30"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="279072975"/>
           <a:ext cx="3705225" cy="180975"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1408,24 +1408,24 @@
       <nvPicPr>
         <cNvPr id="62" name="Imagen 61"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId31"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="283273500"/>
           <a:ext cx="3705225" cy="180975"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1436,7 +1436,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>0</col>
@@ -1454,24 +1454,24 @@
       <nvPicPr>
         <cNvPr id="32" name="Imagen 31"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="61626750"/>
           <a:ext cx="3914775" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1482,7 +1482,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>0</col>
@@ -1500,24 +1500,24 @@
       <nvPicPr>
         <cNvPr id="32" name="Imagen 31"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="98402774"/>
           <a:ext cx="4295775" cy="180975"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1541,24 +1541,24 @@
       <nvPicPr>
         <cNvPr id="33" name="Imagen 32"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="102403275"/>
           <a:ext cx="4295775" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1582,24 +1582,24 @@
       <nvPicPr>
         <cNvPr id="34" name="Imagen 33"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="107365800"/>
           <a:ext cx="4314825" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1623,24 +1623,24 @@
       <nvPicPr>
         <cNvPr id="35" name="Imagen 34"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId4"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="111185325"/>
           <a:ext cx="4295775" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1664,24 +1664,24 @@
       <nvPicPr>
         <cNvPr id="36" name="Imagen 35"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId5"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="113480850"/>
           <a:ext cx="4295775" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1705,24 +1705,24 @@
       <nvPicPr>
         <cNvPr id="37" name="Imagen 36"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId6"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="117119400"/>
           <a:ext cx="4305300" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1746,24 +1746,24 @@
       <nvPicPr>
         <cNvPr id="38" name="Imagen 37"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId7"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="119595900"/>
           <a:ext cx="4295775" cy="190499"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1787,24 +1787,24 @@
       <nvPicPr>
         <cNvPr id="39" name="Imagen 38"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId8"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="125339475"/>
           <a:ext cx="4286250" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1828,24 +1828,24 @@
       <nvPicPr>
         <cNvPr id="40" name="Imagen 39"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId9"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="127996950"/>
           <a:ext cx="4305300" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1869,24 +1869,24 @@
       <nvPicPr>
         <cNvPr id="41" name="Imagen 40"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId10"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="131645026"/>
           <a:ext cx="4295775" cy="180974"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1910,24 +1910,24 @@
       <nvPicPr>
         <cNvPr id="42" name="Imagen 41"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId11"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="136217025"/>
           <a:ext cx="4267200" cy="190499"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1951,24 +1951,24 @@
       <nvPicPr>
         <cNvPr id="43" name="Imagen 42"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId12"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="141370050"/>
           <a:ext cx="4286250" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1992,24 +1992,24 @@
       <nvPicPr>
         <cNvPr id="44" name="Imagen 43"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId13"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="145380075"/>
           <a:ext cx="4305300" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2033,24 +2033,24 @@
       <nvPicPr>
         <cNvPr id="45" name="Imagen 44"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId14"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="147847050"/>
           <a:ext cx="4305300" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2074,24 +2074,24 @@
       <nvPicPr>
         <cNvPr id="46" name="Imagen 45"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId15"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="151504651"/>
           <a:ext cx="4314825" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2115,24 +2115,24 @@
       <nvPicPr>
         <cNvPr id="47" name="Imagen 46"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId16"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="156657676"/>
           <a:ext cx="4295775" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2156,24 +2156,24 @@
       <nvPicPr>
         <cNvPr id="48" name="Imagen 47"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId17"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="159143700"/>
           <a:ext cx="4286250" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2197,24 +2197,24 @@
       <nvPicPr>
         <cNvPr id="49" name="Imagen 48"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId18"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="162572700"/>
           <a:ext cx="4305300" cy="152400"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2238,24 +2238,24 @@
       <nvPicPr>
         <cNvPr id="50" name="Imagen 49"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId19"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="165049201"/>
           <a:ext cx="4305300" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2279,24 +2279,24 @@
       <nvPicPr>
         <cNvPr id="51" name="Imagen 50"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId20"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="168125775"/>
           <a:ext cx="4305300" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2320,24 +2320,24 @@
       <nvPicPr>
         <cNvPr id="52" name="Imagen 51"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId21"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="171926250"/>
           <a:ext cx="4305300" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2361,24 +2361,24 @@
       <nvPicPr>
         <cNvPr id="53" name="Imagen 52"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId22"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="174793276"/>
           <a:ext cx="4295775" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2402,24 +2402,24 @@
       <nvPicPr>
         <cNvPr id="54" name="Imagen 53"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId23"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="179765324"/>
           <a:ext cx="4305300" cy="180975"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2443,24 +2443,24 @@
       <nvPicPr>
         <cNvPr id="55" name="Imagen 54"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId24"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="182241825"/>
           <a:ext cx="4305300" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2471,7 +2471,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>0</col>
@@ -2489,24 +2489,24 @@
       <nvPicPr>
         <cNvPr id="32" name="Imagen 31"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="153390600"/>
           <a:ext cx="4286250" cy="180975"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2530,24 +2530,24 @@
       <nvPicPr>
         <cNvPr id="33" name="Imagen 32"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="166916100"/>
           <a:ext cx="4314825" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2571,24 +2571,24 @@
       <nvPicPr>
         <cNvPr id="34" name="Imagen 33"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId4"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="167125650"/>
           <a:ext cx="4333875" cy="190500"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2612,24 +2612,24 @@
       <nvPicPr>
         <cNvPr id="35" name="Imagen 34"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId5"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="153581100"/>
           <a:ext cx="4276725" cy="190500"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2653,24 +2653,24 @@
       <nvPicPr>
         <cNvPr id="36" name="Imagen 35"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId6"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="169630726"/>
           <a:ext cx="4295775" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2694,24 +2694,24 @@
       <nvPicPr>
         <cNvPr id="37" name="Imagen 36"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId7"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="182394225"/>
           <a:ext cx="4305300" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2735,24 +2735,24 @@
       <nvPicPr>
         <cNvPr id="38" name="Imagen 37"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId8"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="184861201"/>
           <a:ext cx="4295775" cy="142874"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2776,24 +2776,24 @@
       <nvPicPr>
         <cNvPr id="39" name="Imagen 38"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId9"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="189833251"/>
           <a:ext cx="4276725" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2817,24 +2817,24 @@
       <nvPicPr>
         <cNvPr id="40" name="Imagen 39"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId10"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="169830750"/>
           <a:ext cx="4295775" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2858,24 +2858,24 @@
       <nvPicPr>
         <cNvPr id="41" name="Imagen 40"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId11"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="182784751"/>
           <a:ext cx="4314825" cy="180974"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2899,24 +2899,24 @@
       <nvPicPr>
         <cNvPr id="42" name="Imagen 41"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId12"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="185442225"/>
           <a:ext cx="4295775" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2940,24 +2940,24 @@
       <nvPicPr>
         <cNvPr id="43" name="Imagen 42"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId13"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="190014225"/>
           <a:ext cx="4305300" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -2981,24 +2981,24 @@
       <nvPicPr>
         <cNvPr id="44" name="Imagen 43"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId14"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="197653275"/>
           <a:ext cx="4295775" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3022,24 +3022,24 @@
       <nvPicPr>
         <cNvPr id="45" name="Imagen 44"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId15"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="212493225"/>
           <a:ext cx="4286250" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3063,24 +3063,24 @@
       <nvPicPr>
         <cNvPr id="46" name="Imagen 45"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId16"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="197919975"/>
           <a:ext cx="4305300" cy="152400"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3104,24 +3104,24 @@
       <nvPicPr>
         <cNvPr id="47" name="Imagen 46"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId17"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="214674451"/>
           <a:ext cx="4295775" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3145,24 +3145,24 @@
       <nvPicPr>
         <cNvPr id="48" name="Imagen 47"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId18"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="225723450"/>
           <a:ext cx="4286250" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3186,24 +3186,24 @@
       <nvPicPr>
         <cNvPr id="49" name="Imagen 48"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId19"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="225942525"/>
           <a:ext cx="4286250" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3227,24 +3227,24 @@
       <nvPicPr>
         <cNvPr id="50" name="Imagen 49"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId20"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="228619050"/>
           <a:ext cx="4305300" cy="152399"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3268,24 +3268,24 @@
       <nvPicPr>
         <cNvPr id="51" name="Imagen 50"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId21"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="244621050"/>
           <a:ext cx="4305300" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3309,24 +3309,24 @@
       <nvPicPr>
         <cNvPr id="52" name="Imagen 51"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId22"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="244430549"/>
           <a:ext cx="4314825" cy="192197"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3350,24 +3350,24 @@
       <nvPicPr>
         <cNvPr id="53" name="Imagen 52"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId23"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="228428551"/>
           <a:ext cx="4305300" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3391,24 +3391,24 @@
       <nvPicPr>
         <cNvPr id="54" name="Imagen 53"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId24"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="261023101"/>
           <a:ext cx="4295775" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3432,24 +3432,24 @@
       <nvPicPr>
         <cNvPr id="55" name="Imagen 54"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId25"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="246735600"/>
           <a:ext cx="4305300" cy="152400"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3473,24 +3473,24 @@
       <nvPicPr>
         <cNvPr id="56" name="Imagen 55"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId26"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="261251700"/>
           <a:ext cx="4295775" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3514,24 +3514,24 @@
       <nvPicPr>
         <cNvPr id="57" name="Imagen 56"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId27"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="282425775"/>
           <a:ext cx="4305300" cy="152400"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3555,24 +3555,24 @@
       <nvPicPr>
         <cNvPr id="58" name="Imagen 57"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId28"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="277672801"/>
           <a:ext cx="4295775" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3596,24 +3596,24 @@
       <nvPicPr>
         <cNvPr id="59" name="Imagen 58"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId29"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="275186774"/>
           <a:ext cx="4305300" cy="180975"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3637,24 +3637,24 @@
       <nvPicPr>
         <cNvPr id="60" name="Imagen 59"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId30"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="264137775"/>
           <a:ext cx="4314825" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3678,24 +3678,24 @@
       <nvPicPr>
         <cNvPr id="61" name="Imagen 60"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId31"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="278063325"/>
           <a:ext cx="4295775" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3719,24 +3719,24 @@
       <nvPicPr>
         <cNvPr id="62" name="Imagen 61"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId32"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="275596350"/>
           <a:ext cx="4314825" cy="152399"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3760,24 +3760,24 @@
       <nvPicPr>
         <cNvPr id="63" name="Imagen 62"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId33"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="264347325"/>
           <a:ext cx="4314825" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3801,24 +3801,24 @@
       <nvPicPr>
         <cNvPr id="64" name="Imagen 63"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId34"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="289874325"/>
           <a:ext cx="4286250" cy="152400"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3842,24 +3842,24 @@
       <nvPicPr>
         <cNvPr id="65" name="Imagen 64"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId35"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="303780826"/>
           <a:ext cx="4295775" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3883,24 +3883,24 @@
       <nvPicPr>
         <cNvPr id="67" name="Imagen 66"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId36"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="290283900"/>
           <a:ext cx="4267200" cy="180975"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3924,24 +3924,24 @@
       <nvPicPr>
         <cNvPr id="66" name="Imagen 65"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId37"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="306352575"/>
           <a:ext cx="4305300" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -3965,24 +3965,24 @@
       <nvPicPr>
         <cNvPr id="68" name="Imagen 67"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId38"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="324450076"/>
           <a:ext cx="4286250" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4006,24 +4006,24 @@
       <nvPicPr>
         <cNvPr id="69" name="Imagen 68"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId39"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="324650100"/>
           <a:ext cx="4295775" cy="180974"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4047,24 +4047,24 @@
       <nvPicPr>
         <cNvPr id="70" name="Imagen 69"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId40"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="306752625"/>
           <a:ext cx="4324350" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4088,24 +4088,24 @@
       <nvPicPr>
         <cNvPr id="71" name="Imagen 70"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId41"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="304266600"/>
           <a:ext cx="4295775" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4129,24 +4129,24 @@
       <nvPicPr>
         <cNvPr id="72" name="Imagen 71"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId42"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="332365350"/>
           <a:ext cx="4305300" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4170,24 +4170,24 @@
       <nvPicPr>
         <cNvPr id="73" name="Imagen 72"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId43"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="358073325"/>
           <a:ext cx="4286250" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4211,24 +4211,24 @@
       <nvPicPr>
         <cNvPr id="74" name="Imagen 73"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId44"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="332555850"/>
           <a:ext cx="4324350" cy="180975"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4252,24 +4252,24 @@
       <nvPicPr>
         <cNvPr id="75" name="Imagen 74"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId45"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="358463850"/>
           <a:ext cx="4276725" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4293,24 +4293,24 @@
       <nvPicPr>
         <cNvPr id="76" name="Imagen 75"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId46"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="360778425"/>
           <a:ext cx="4295775" cy="190499"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4334,24 +4334,24 @@
       <nvPicPr>
         <cNvPr id="77" name="Imagen 76"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId47"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="374884950"/>
           <a:ext cx="4295775" cy="152399"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4375,24 +4375,24 @@
       <nvPicPr>
         <cNvPr id="78" name="Imagen 77"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId48"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="377542425"/>
           <a:ext cx="4295775" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4416,24 +4416,24 @@
       <nvPicPr>
         <cNvPr id="79" name="Imagen 78"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId49"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="390296400"/>
           <a:ext cx="4314825" cy="190499"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4457,24 +4457,24 @@
       <nvPicPr>
         <cNvPr id="80" name="Imagen 79"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId50"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="375265950"/>
           <a:ext cx="4295775" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4498,24 +4498,24 @@
       <nvPicPr>
         <cNvPr id="81" name="Imagen 80"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId51"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="378132975"/>
           <a:ext cx="4295775" cy="152399"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4539,24 +4539,24 @@
       <nvPicPr>
         <cNvPr id="82" name="Imagen 81"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId52"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="391086975"/>
           <a:ext cx="4295775" cy="164913"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4580,24 +4580,24 @@
       <nvPicPr>
         <cNvPr id="83" name="Imagen 82"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId53"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="361007024"/>
           <a:ext cx="4286250" cy="142875"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4621,24 +4621,24 @@
       <nvPicPr>
         <cNvPr id="84" name="Imagen 83"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId54"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="399678526"/>
           <a:ext cx="4305300" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4662,24 +4662,24 @@
       <nvPicPr>
         <cNvPr id="85" name="Imagen 84"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId55"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="419528625"/>
           <a:ext cx="4305300" cy="190500"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4703,24 +4703,24 @@
       <nvPicPr>
         <cNvPr id="86" name="Imagen 85"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId56"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="419728650"/>
           <a:ext cx="4314825" cy="152399"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4744,24 +4744,24 @@
       <nvPicPr>
         <cNvPr id="87" name="Imagen 86"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId57"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="399888075"/>
           <a:ext cx="4314825" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4785,24 +4785,24 @@
       <nvPicPr>
         <cNvPr id="88" name="Imagen 87"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId58"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="463000725"/>
           <a:ext cx="4276725" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4826,24 +4826,24 @@
       <nvPicPr>
         <cNvPr id="89" name="Imagen 88"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId59"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="422233725"/>
           <a:ext cx="4295775" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4867,24 +4867,24 @@
       <nvPicPr>
         <cNvPr id="90" name="Imagen 89"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId60"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId60"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="463210276"/>
           <a:ext cx="4305300" cy="161924"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4908,24 +4908,24 @@
       <nvPicPr>
         <cNvPr id="91" name="Imagen 90"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId61"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId61"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="470468325"/>
           <a:ext cx="4305300" cy="152399"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4949,24 +4949,24 @@
       <nvPicPr>
         <cNvPr id="92" name="Imagen 91"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId62"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId62"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="470639775"/>
           <a:ext cx="4295775" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -4990,24 +4990,24 @@
       <nvPicPr>
         <cNvPr id="93" name="Imagen 92"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId63"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId63"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="472935300"/>
           <a:ext cx="4305300" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5031,24 +5031,24 @@
       <nvPicPr>
         <cNvPr id="94" name="Imagen 93"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId64"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId64"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="484412925"/>
           <a:ext cx="4286250" cy="180975"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5072,24 +5072,24 @@
       <nvPicPr>
         <cNvPr id="95" name="Imagen 94"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId65"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId65"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="473144850"/>
           <a:ext cx="4295775" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5113,24 +5113,24 @@
       <nvPicPr>
         <cNvPr id="96" name="Imagen 95"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId66"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId66"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="487689526"/>
           <a:ext cx="4286250" cy="152400"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5154,24 +5154,24 @@
       <nvPicPr>
         <cNvPr id="97" name="Imagen 96"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId67"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId67"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="499081425"/>
           <a:ext cx="4295775" cy="190500"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5195,24 +5195,24 @@
       <nvPicPr>
         <cNvPr id="98" name="Imagen 97"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId68"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId68"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="501176925"/>
           <a:ext cx="4305300" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5236,24 +5236,24 @@
       <nvPicPr>
         <cNvPr id="99" name="Imagen 98"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId69"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId69"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="506139450"/>
           <a:ext cx="4276725" cy="162649"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5277,24 +5277,24 @@
       <nvPicPr>
         <cNvPr id="100" name="Imagen 99"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId70"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId70"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="484612950"/>
           <a:ext cx="4286249" cy="171450"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5318,24 +5318,24 @@
       <nvPicPr>
         <cNvPr id="101" name="Imagen 100"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId71"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId71"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="499490999"/>
           <a:ext cx="4314825" cy="153203"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5359,24 +5359,24 @@
       <nvPicPr>
         <cNvPr id="102" name="Imagen 101"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId72"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId72"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="501767474"/>
           <a:ext cx="4324350" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5400,24 +5400,24 @@
       <nvPicPr>
         <cNvPr id="103" name="Imagen 102"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId73"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId73"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="506910975"/>
           <a:ext cx="4305300" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5441,24 +5441,24 @@
       <nvPicPr>
         <cNvPr id="104" name="Imagen 103"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId74"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId74"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="510540001"/>
           <a:ext cx="4305300" cy="152400"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5482,24 +5482,24 @@
       <nvPicPr>
         <cNvPr id="106" name="Imagen 105"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId75"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId75"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="524132175"/>
           <a:ext cx="4305300" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5518,24 +5518,24 @@
       <nvPicPr>
         <cNvPr id="105" name="Imagen 104"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="487699050"/>
           <a:ext cx="4286250" cy="180975"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5546,7 +5546,7 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>0</col>
@@ -5564,24 +5564,24 @@
       <nvPicPr>
         <cNvPr id="32" name="Imagen 31"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="82257900"/>
           <a:ext cx="4295775" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5605,24 +5605,24 @@
       <nvPicPr>
         <cNvPr id="33" name="Imagen 32"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="84353399"/>
           <a:ext cx="4295775" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5646,24 +5646,24 @@
       <nvPicPr>
         <cNvPr id="34" name="Imagen 33"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="87401400"/>
           <a:ext cx="4267200" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5687,24 +5687,24 @@
       <nvPicPr>
         <cNvPr id="35" name="Imagen 34"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId4"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="89325450"/>
           <a:ext cx="4324350" cy="163727"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5728,24 +5728,24 @@
       <nvPicPr>
         <cNvPr id="36" name="Imagen 35"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId5"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="91992451"/>
           <a:ext cx="4286249" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5769,24 +5769,24 @@
       <nvPicPr>
         <cNvPr id="37" name="Imagen 36"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId6"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="94106999"/>
           <a:ext cx="4295775" cy="180975"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -5797,7 +5797,7 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>0</col>
@@ -5815,24 +5815,24 @@
       <nvPicPr>
         <cNvPr id="32" name="Imagen 31"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="1" y="62798325"/>
           <a:ext cx="4286250" cy="171449"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -6138,7 +6138,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor theme="8"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6381,7 +6381,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7026,7 +7026,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor theme="8"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -7694,7 +7694,7 @@
     <row r="483" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12930,7 +12930,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B6"/>
+  <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
       <selection activeCell="A313" sqref="A313"/>
@@ -13005,6 +13005,18 @@
       <c r="B6" t="inlineStr">
         <is>
           <t>112863722</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CCAJ-LP08/51/23</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>112865831</t>
         </is>
       </c>
     </row>
@@ -16353,7 +16365,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor theme="8"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -16977,7 +16989,7 @@
     <row r="319" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17830,7 +17842,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor theme="9"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -17949,12 +17961,12 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor theme="8"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -18732,7 +18744,7 @@
     <row r="939" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -19376,7 +19388,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor theme="8"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -20371,7 +20383,7 @@
     <row r="2675" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>